<commit_message>
Add request detail when upload SO or UQ input
</commit_message>
<xml_diff>
--- a/NMVS/uploads/IDL01_Item data list.xlsx
+++ b/NMVS/uploads/IDL01_Item data list.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/276815161ec3e88f/Working Space/Netmarks/Aica/Aica Docs/AICA001_Item data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="26" documentId="10_ncr:80_{941C12A3-ADD2-4F0F-9B20-1A74F4055260}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BBAD1539-72F5-43CA-981F-C75C6819322E}"/>
+  <xr:revisionPtr revIDLastSave="29" documentId="10_ncr:80_{941C12A3-ADD2-4F0F-9B20-1A74F4055260}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3B59B18B-37E2-4F13-A002-AC07CC97F076}"/>
   <bookViews>
-    <workbookView xWindow="2775" yWindow="4185" windowWidth="21600" windowHeight="11295" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6558" uniqueCount="2096">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6557" uniqueCount="2095">
   <si>
     <t>FG-01-4110-1-1200-0</t>
   </si>
@@ -6322,10 +6322,7 @@
     <t>12</t>
   </si>
   <si>
-    <t>Tax</t>
-  </si>
-  <si>
-    <t>Warehouse space (per 1 pack)##</t>
+    <t>Warehouse space (per 1 pack)</t>
   </si>
 </sst>
 </file>
@@ -6430,7 +6427,7 @@
       <alignment vertical="top"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="top"/>
     </xf>
@@ -6453,9 +6450,6 @@
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -6871,11 +6865,11 @@
     <outlinePr summaryBelow="0"/>
     <pageSetUpPr autoPageBreaks="0"/>
   </sheetPr>
-  <dimension ref="A1:G1237"/>
+  <dimension ref="A1:F1237"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F2" sqref="F2"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A30" sqref="A30:B41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.85546875" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -6888,17 +6882,17 @@
     <col min="7" max="7" width="27.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="20.25" x14ac:dyDescent="0.2">
-      <c r="A1" s="9" t="s">
+    <row r="1" spans="1:6" ht="20.25" x14ac:dyDescent="0.2">
+      <c r="A1" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
         <v>3</v>
       </c>
@@ -6915,13 +6909,10 @@
         <v>7</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>2095</v>
-      </c>
-      <c r="G2" s="8" t="s">
         <v>2094</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -6941,7 +6932,7 @@
         <v>2085</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -6961,7 +6952,7 @@
         <v>2085</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -6981,7 +6972,7 @@
         <v>2085</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>13</v>
       </c>
@@ -7001,7 +6992,7 @@
         <v>2085</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>15</v>
       </c>
@@ -7021,7 +7012,7 @@
         <v>2085</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>17</v>
       </c>
@@ -7041,7 +7032,7 @@
         <v>2085</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>19</v>
       </c>
@@ -7061,7 +7052,7 @@
         <v>2085</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>21</v>
       </c>
@@ -7081,7 +7072,7 @@
         <v>2085</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>23</v>
       </c>
@@ -7101,7 +7092,7 @@
         <v>2086</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>25</v>
       </c>
@@ -7121,7 +7112,7 @@
         <v>2086</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>29</v>
       </c>
@@ -7141,7 +7132,7 @@
         <v>2087</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>30</v>
       </c>
@@ -7161,7 +7152,7 @@
         <v>2087</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>31</v>
       </c>
@@ -7181,7 +7172,7 @@
         <v>2087</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>32</v>
       </c>
@@ -28786,7 +28777,7 @@
       <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
       <pageSetup paperSize="9" fitToWidth="0" fitToHeight="0" orientation="landscape" r:id="rId1"/>
       <headerFooter alignWithMargins="0"/>
-      <autoFilter ref="A2:F2" xr:uid="{23A271F7-BAE9-498D-9F9A-54CFD0A5DA94}"/>
+      <autoFilter ref="A2:F2" xr:uid="{39268521-391D-42E2-A536-E44D4AFFEF9D}"/>
     </customSheetView>
   </customSheetViews>
   <mergeCells count="1">

</xml_diff>

<commit_message>
New issue order, complete issue to MFG
</commit_message>
<xml_diff>
--- a/NMVS/uploads/IDL01_Item data list.xlsx
+++ b/NMVS/uploads/IDL01_Item data list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/276815161ec3e88f/Working Space/Netmarks/Aica/Aica Docs/AICA001_Item data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="229" documentId="10_ncr:80_{941C12A3-ADD2-4F0F-9B20-1A74F4055260}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E4F62076-DD76-454F-9959-98977F031352}"/>
+  <xr:revisionPtr revIDLastSave="251" documentId="10_ncr:80_{941C12A3-ADD2-4F0F-9B20-1A74F4055260}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DD7D6198-3BCB-400F-B834-1B6DA606D17C}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6360" uniqueCount="2097">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5991" uniqueCount="2106">
   <si>
     <t>FG-01-4110-1-1200-0</t>
   </si>
@@ -6329,6 +6329,33 @@
   </si>
   <si>
     <t>FLEXI</t>
+  </si>
+  <si>
+    <t>17KG/CAN (LUTENSOL ON60</t>
+  </si>
+  <si>
+    <t>METHANO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dau </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> POC701</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> POC702</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> POC703</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> POC704</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> POC705</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> POC706</t>
   </si>
 </sst>
 </file>
@@ -6874,8 +6901,8 @@
   <dimension ref="A1:F1237"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A933" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E955" sqref="E955"/>
+      <pane ySplit="2" topLeftCell="A1068" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G1086" sqref="G1086"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.85546875" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -25302,11 +25329,12 @@
       <c r="D922" t="s">
         <v>2084</v>
       </c>
-      <c r="E922" t="s">
-        <v>2088</v>
-      </c>
-      <c r="F922" t="s">
-        <v>2088</v>
+      <c r="E922">
+        <v>17</v>
+      </c>
+      <c r="F922">
+        <f>E922</f>
+        <v>17</v>
       </c>
     </row>
     <row r="923" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -25322,11 +25350,12 @@
       <c r="D923" t="s">
         <v>2084</v>
       </c>
-      <c r="E923" t="s">
-        <v>2088</v>
-      </c>
-      <c r="F923" t="s">
-        <v>2088</v>
+      <c r="E923">
+        <v>18</v>
+      </c>
+      <c r="F923">
+        <f t="shared" ref="F923:F986" si="0">E923</f>
+        <v>18</v>
       </c>
     </row>
     <row r="924" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -25342,11 +25371,12 @@
       <c r="D924" t="s">
         <v>2084</v>
       </c>
-      <c r="E924" t="s">
-        <v>2088</v>
-      </c>
-      <c r="F924" t="s">
-        <v>2088</v>
+      <c r="E924">
+        <v>17</v>
+      </c>
+      <c r="F924">
+        <f t="shared" si="0"/>
+        <v>17</v>
       </c>
     </row>
     <row r="925" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -25362,11 +25392,12 @@
       <c r="D925" t="s">
         <v>2084</v>
       </c>
-      <c r="E925" t="s">
-        <v>2088</v>
-      </c>
-      <c r="F925" t="s">
-        <v>2088</v>
+      <c r="E925">
+        <v>16</v>
+      </c>
+      <c r="F925">
+        <f t="shared" si="0"/>
+        <v>16</v>
       </c>
     </row>
     <row r="926" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -25382,11 +25413,12 @@
       <c r="D926" t="s">
         <v>2084</v>
       </c>
-      <c r="E926" t="s">
-        <v>2088</v>
-      </c>
-      <c r="F926" t="s">
-        <v>2088</v>
+      <c r="E926">
+        <v>18</v>
+      </c>
+      <c r="F926">
+        <f t="shared" si="0"/>
+        <v>18</v>
       </c>
     </row>
     <row r="927" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -25402,11 +25434,12 @@
       <c r="D927" t="s">
         <v>2084</v>
       </c>
-      <c r="E927" t="s">
-        <v>2088</v>
-      </c>
-      <c r="F927" t="s">
-        <v>2088</v>
+      <c r="E927">
+        <v>16</v>
+      </c>
+      <c r="F927">
+        <f t="shared" si="0"/>
+        <v>16</v>
       </c>
     </row>
     <row r="928" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -25422,11 +25455,12 @@
       <c r="D928" t="s">
         <v>2084</v>
       </c>
-      <c r="E928" t="s">
-        <v>2088</v>
-      </c>
-      <c r="F928" t="s">
-        <v>2088</v>
+      <c r="E928">
+        <v>15</v>
+      </c>
+      <c r="F928">
+        <f t="shared" si="0"/>
+        <v>15</v>
       </c>
     </row>
     <row r="929" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -25442,11 +25476,12 @@
       <c r="D929" t="s">
         <v>2092</v>
       </c>
-      <c r="E929" t="s">
-        <v>2088</v>
-      </c>
-      <c r="F929" t="s">
-        <v>2088</v>
+      <c r="E929">
+        <v>16</v>
+      </c>
+      <c r="F929">
+        <f t="shared" si="0"/>
+        <v>16</v>
       </c>
     </row>
     <row r="930" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -25462,11 +25497,12 @@
       <c r="D930" t="s">
         <v>2092</v>
       </c>
-      <c r="E930" t="s">
-        <v>2088</v>
-      </c>
-      <c r="F930" t="s">
-        <v>2088</v>
+      <c r="E930">
+        <v>16</v>
+      </c>
+      <c r="F930">
+        <f t="shared" si="0"/>
+        <v>16</v>
       </c>
     </row>
     <row r="931" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -25482,11 +25518,12 @@
       <c r="D931" t="s">
         <v>2092</v>
       </c>
-      <c r="E931" t="s">
-        <v>2088</v>
-      </c>
-      <c r="F931" t="s">
-        <v>2088</v>
+      <c r="E931">
+        <v>15</v>
+      </c>
+      <c r="F931">
+        <f t="shared" si="0"/>
+        <v>15</v>
       </c>
     </row>
     <row r="932" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -25502,11 +25539,12 @@
       <c r="D932" t="s">
         <v>2091</v>
       </c>
-      <c r="E932" t="s">
-        <v>2088</v>
-      </c>
-      <c r="F932" t="s">
-        <v>2088</v>
+      <c r="E932">
+        <v>15</v>
+      </c>
+      <c r="F932">
+        <f t="shared" si="0"/>
+        <v>15</v>
       </c>
     </row>
     <row r="933" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -25522,11 +25560,12 @@
       <c r="D933" t="s">
         <v>2092</v>
       </c>
-      <c r="E933" t="s">
-        <v>2088</v>
-      </c>
-      <c r="F933" t="s">
-        <v>2088</v>
+      <c r="E933">
+        <v>16</v>
+      </c>
+      <c r="F933">
+        <f t="shared" si="0"/>
+        <v>16</v>
       </c>
     </row>
     <row r="934" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -25545,8 +25584,9 @@
       <c r="E934" t="s">
         <v>2090</v>
       </c>
-      <c r="F934" t="s">
-        <v>2090</v>
+      <c r="F934" t="str">
+        <f t="shared" si="0"/>
+        <v>20</v>
       </c>
     </row>
     <row r="935" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -25562,11 +25602,12 @@
       <c r="D935" t="s">
         <v>2084</v>
       </c>
-      <c r="E935" t="s">
-        <v>2088</v>
-      </c>
-      <c r="F935" t="s">
-        <v>2088</v>
+      <c r="E935">
+        <v>25</v>
+      </c>
+      <c r="F935">
+        <f t="shared" si="0"/>
+        <v>25</v>
       </c>
     </row>
     <row r="936" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -25585,8 +25626,9 @@
       <c r="E936" t="s">
         <v>2090</v>
       </c>
-      <c r="F936" t="s">
-        <v>2090</v>
+      <c r="F936" t="str">
+        <f t="shared" si="0"/>
+        <v>20</v>
       </c>
     </row>
     <row r="937" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -25602,11 +25644,12 @@
       <c r="D937" t="s">
         <v>27</v>
       </c>
-      <c r="E937" t="s">
-        <v>2088</v>
-      </c>
-      <c r="F937" t="s">
-        <v>2088</v>
+      <c r="E937">
+        <v>190</v>
+      </c>
+      <c r="F937">
+        <f t="shared" si="0"/>
+        <v>190</v>
       </c>
     </row>
     <row r="938" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -25625,8 +25668,9 @@
       <c r="E938" t="s">
         <v>2090</v>
       </c>
-      <c r="F938" t="s">
-        <v>2090</v>
+      <c r="F938" t="str">
+        <f t="shared" si="0"/>
+        <v>20</v>
       </c>
     </row>
     <row r="939" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -25645,8 +25689,9 @@
       <c r="E939" t="s">
         <v>2090</v>
       </c>
-      <c r="F939" t="s">
-        <v>2090</v>
+      <c r="F939" t="str">
+        <f t="shared" si="0"/>
+        <v>20</v>
       </c>
     </row>
     <row r="940" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -25665,8 +25710,9 @@
       <c r="E940" t="s">
         <v>2090</v>
       </c>
-      <c r="F940" t="s">
-        <v>2090</v>
+      <c r="F940" t="str">
+        <f t="shared" si="0"/>
+        <v>20</v>
       </c>
     </row>
     <row r="941" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -25685,8 +25731,9 @@
       <c r="E941" t="s">
         <v>2090</v>
       </c>
-      <c r="F941" t="s">
-        <v>2090</v>
+      <c r="F941" t="str">
+        <f t="shared" si="0"/>
+        <v>20</v>
       </c>
     </row>
     <row r="942" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -25705,8 +25752,9 @@
       <c r="E942" t="s">
         <v>2090</v>
       </c>
-      <c r="F942" t="s">
-        <v>2090</v>
+      <c r="F942" t="str">
+        <f t="shared" si="0"/>
+        <v>20</v>
       </c>
     </row>
     <row r="943" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -25723,10 +25771,11 @@
         <v>2084</v>
       </c>
       <c r="E943">
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="F943">
-        <v>1</v>
+        <f t="shared" si="0"/>
+        <v>18</v>
       </c>
     </row>
     <row r="944" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -25743,10 +25792,11 @@
         <v>27</v>
       </c>
       <c r="E944">
-        <v>1</v>
+        <v>180</v>
       </c>
       <c r="F944">
-        <v>1</v>
+        <f t="shared" si="0"/>
+        <v>180</v>
       </c>
     </row>
     <row r="945" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -25763,10 +25813,11 @@
         <v>2092</v>
       </c>
       <c r="E945">
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="F945">
-        <v>1</v>
+        <f t="shared" si="0"/>
+        <v>18</v>
       </c>
     </row>
     <row r="946" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -25783,10 +25834,11 @@
         <v>27</v>
       </c>
       <c r="E946">
-        <v>1</v>
+        <v>170</v>
       </c>
       <c r="F946">
-        <v>1</v>
+        <f t="shared" si="0"/>
+        <v>170</v>
       </c>
     </row>
     <row r="947" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -25805,8 +25857,9 @@
       <c r="E947" t="s">
         <v>2090</v>
       </c>
-      <c r="F947" t="s">
-        <v>2090</v>
+      <c r="F947" t="str">
+        <f t="shared" si="0"/>
+        <v>20</v>
       </c>
     </row>
     <row r="948" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -25823,10 +25876,11 @@
         <v>27</v>
       </c>
       <c r="E948">
-        <v>1</v>
+        <v>180</v>
       </c>
       <c r="F948">
-        <v>1</v>
+        <f t="shared" si="0"/>
+        <v>180</v>
       </c>
     </row>
     <row r="949" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -25846,6 +25900,7 @@
         <v>1</v>
       </c>
       <c r="F949">
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -25866,6 +25921,7 @@
         <v>1</v>
       </c>
       <c r="F950">
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -25885,8 +25941,9 @@
       <c r="E951" t="s">
         <v>2090</v>
       </c>
-      <c r="F951" t="s">
-        <v>2090</v>
+      <c r="F951" t="str">
+        <f>E951</f>
+        <v>20</v>
       </c>
     </row>
     <row r="952" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -25905,8 +25962,9 @@
       <c r="E952" t="s">
         <v>2090</v>
       </c>
-      <c r="F952" t="s">
-        <v>2090</v>
+      <c r="F952" t="str">
+        <f t="shared" si="0"/>
+        <v>20</v>
       </c>
     </row>
     <row r="953" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -25926,6 +25984,7 @@
         <v>180</v>
       </c>
       <c r="F953">
+        <f t="shared" si="0"/>
         <v>180</v>
       </c>
     </row>
@@ -25946,6 +26005,7 @@
         <v>180</v>
       </c>
       <c r="F954">
+        <f t="shared" si="0"/>
         <v>180</v>
       </c>
     </row>
@@ -25965,8 +26025,9 @@
       <c r="E955" t="s">
         <v>2089</v>
       </c>
-      <c r="F955" t="s">
-        <v>2089</v>
+      <c r="F955" t="str">
+        <f t="shared" si="0"/>
+        <v>10</v>
       </c>
     </row>
     <row r="956" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -25985,8 +26046,9 @@
       <c r="E956" t="s">
         <v>2089</v>
       </c>
-      <c r="F956" t="s">
-        <v>2089</v>
+      <c r="F956" t="str">
+        <f t="shared" si="0"/>
+        <v>10</v>
       </c>
     </row>
     <row r="957" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -26002,11 +26064,12 @@
       <c r="D957" t="s">
         <v>2084</v>
       </c>
-      <c r="E957" t="s">
-        <v>2088</v>
-      </c>
-      <c r="F957" t="s">
-        <v>2088</v>
+      <c r="E957">
+        <v>15</v>
+      </c>
+      <c r="F957">
+        <f t="shared" si="0"/>
+        <v>15</v>
       </c>
     </row>
     <row r="958" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -26025,8 +26088,9 @@
       <c r="E958" t="s">
         <v>2090</v>
       </c>
-      <c r="F958" t="s">
-        <v>2090</v>
+      <c r="F958" t="str">
+        <f t="shared" si="0"/>
+        <v>20</v>
       </c>
     </row>
     <row r="959" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -26045,8 +26109,9 @@
       <c r="E959" t="s">
         <v>2090</v>
       </c>
-      <c r="F959" t="s">
-        <v>2090</v>
+      <c r="F959" t="str">
+        <f t="shared" si="0"/>
+        <v>20</v>
       </c>
     </row>
     <row r="960" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -26062,11 +26127,12 @@
       <c r="D960" t="s">
         <v>2084</v>
       </c>
-      <c r="E960" t="s">
-        <v>2088</v>
-      </c>
-      <c r="F960" t="s">
-        <v>2088</v>
+      <c r="E960">
+        <v>15</v>
+      </c>
+      <c r="F960">
+        <f t="shared" si="0"/>
+        <v>15</v>
       </c>
     </row>
     <row r="961" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -26085,8 +26151,9 @@
       <c r="E961" t="s">
         <v>2089</v>
       </c>
-      <c r="F961" t="s">
-        <v>2089</v>
+      <c r="F961" t="str">
+        <f t="shared" si="0"/>
+        <v>10</v>
       </c>
     </row>
     <row r="962" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -26105,8 +26172,9 @@
       <c r="E962" t="s">
         <v>2089</v>
       </c>
-      <c r="F962" t="s">
-        <v>2089</v>
+      <c r="F962" t="str">
+        <f t="shared" si="0"/>
+        <v>10</v>
       </c>
     </row>
     <row r="963" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -26125,8 +26193,9 @@
       <c r="E963" t="s">
         <v>2089</v>
       </c>
-      <c r="F963" t="s">
-        <v>2089</v>
+      <c r="F963" t="str">
+        <f t="shared" si="0"/>
+        <v>10</v>
       </c>
     </row>
     <row r="964" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -26145,8 +26214,9 @@
       <c r="E964" t="s">
         <v>2090</v>
       </c>
-      <c r="F964" t="s">
-        <v>2090</v>
+      <c r="F964" t="str">
+        <f t="shared" si="0"/>
+        <v>20</v>
       </c>
     </row>
     <row r="965" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -26162,11 +26232,12 @@
       <c r="D965" t="s">
         <v>2084</v>
       </c>
-      <c r="E965" t="s">
-        <v>2088</v>
-      </c>
-      <c r="F965" t="s">
-        <v>2088</v>
+      <c r="E965">
+        <v>15</v>
+      </c>
+      <c r="F965">
+        <f t="shared" si="0"/>
+        <v>15</v>
       </c>
     </row>
     <row r="966" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -26185,8 +26256,9 @@
       <c r="E966" t="s">
         <v>2089</v>
       </c>
-      <c r="F966" t="s">
-        <v>2089</v>
+      <c r="F966" t="str">
+        <f t="shared" si="0"/>
+        <v>10</v>
       </c>
     </row>
     <row r="967" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -26205,8 +26277,9 @@
       <c r="E967" t="s">
         <v>2090</v>
       </c>
-      <c r="F967" t="s">
-        <v>2090</v>
+      <c r="F967" t="str">
+        <f t="shared" si="0"/>
+        <v>20</v>
       </c>
     </row>
     <row r="968" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -26222,11 +26295,12 @@
       <c r="D968" t="s">
         <v>2091</v>
       </c>
-      <c r="E968" t="s">
-        <v>2088</v>
-      </c>
-      <c r="F968" t="s">
-        <v>2088</v>
+      <c r="E968">
+        <v>1</v>
+      </c>
+      <c r="F968">
+        <f t="shared" si="0"/>
+        <v>1</v>
       </c>
     </row>
     <row r="969" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -26245,8 +26319,9 @@
       <c r="E969" t="s">
         <v>2090</v>
       </c>
-      <c r="F969" t="s">
-        <v>2090</v>
+      <c r="F969" t="str">
+        <f t="shared" si="0"/>
+        <v>20</v>
       </c>
     </row>
     <row r="970" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -26265,8 +26340,9 @@
       <c r="E970" t="s">
         <v>2089</v>
       </c>
-      <c r="F970" t="s">
-        <v>2089</v>
+      <c r="F970" t="str">
+        <f t="shared" si="0"/>
+        <v>10</v>
       </c>
     </row>
     <row r="971" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -26282,11 +26358,12 @@
       <c r="D971" t="s">
         <v>2091</v>
       </c>
-      <c r="E971" t="s">
-        <v>2088</v>
-      </c>
-      <c r="F971" t="s">
-        <v>2088</v>
+      <c r="E971">
+        <v>25</v>
+      </c>
+      <c r="F971">
+        <f t="shared" si="0"/>
+        <v>25</v>
       </c>
     </row>
     <row r="972" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -26302,11 +26379,12 @@
       <c r="D972" t="s">
         <v>2091</v>
       </c>
-      <c r="E972" t="s">
-        <v>2088</v>
-      </c>
-      <c r="F972" t="s">
-        <v>2088</v>
+      <c r="E972">
+        <v>25</v>
+      </c>
+      <c r="F972">
+        <f t="shared" si="0"/>
+        <v>25</v>
       </c>
     </row>
     <row r="973" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -26325,8 +26403,9 @@
       <c r="E973" t="s">
         <v>2090</v>
       </c>
-      <c r="F973" t="s">
-        <v>2090</v>
+      <c r="F973" t="str">
+        <f t="shared" si="0"/>
+        <v>20</v>
       </c>
     </row>
     <row r="974" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -26345,8 +26424,9 @@
       <c r="E974" t="s">
         <v>2090</v>
       </c>
-      <c r="F974" t="s">
-        <v>2090</v>
+      <c r="F974" t="str">
+        <f t="shared" si="0"/>
+        <v>20</v>
       </c>
     </row>
     <row r="975" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -26365,8 +26445,9 @@
       <c r="E975" t="s">
         <v>2090</v>
       </c>
-      <c r="F975" t="s">
-        <v>2090</v>
+      <c r="F975" t="str">
+        <f t="shared" si="0"/>
+        <v>20</v>
       </c>
     </row>
     <row r="976" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -26385,8 +26466,9 @@
       <c r="E976" t="s">
         <v>2090</v>
       </c>
-      <c r="F976" t="s">
-        <v>2090</v>
+      <c r="F976" t="str">
+        <f>E976</f>
+        <v>20</v>
       </c>
     </row>
     <row r="977" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -26402,11 +26484,12 @@
       <c r="D977" t="s">
         <v>27</v>
       </c>
-      <c r="E977" t="s">
-        <v>2088</v>
-      </c>
-      <c r="F977" t="s">
-        <v>2088</v>
+      <c r="E977">
+        <v>180</v>
+      </c>
+      <c r="F977">
+        <f t="shared" si="0"/>
+        <v>180</v>
       </c>
     </row>
     <row r="978" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -26425,8 +26508,9 @@
       <c r="E978" t="s">
         <v>2090</v>
       </c>
-      <c r="F978" t="s">
-        <v>2090</v>
+      <c r="F978" t="str">
+        <f t="shared" si="0"/>
+        <v>20</v>
       </c>
     </row>
     <row r="979" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -26442,11 +26526,12 @@
       <c r="D979" t="s">
         <v>2084</v>
       </c>
-      <c r="E979" t="s">
-        <v>2088</v>
-      </c>
-      <c r="F979" t="s">
-        <v>2088</v>
+      <c r="E979">
+        <v>35</v>
+      </c>
+      <c r="F979">
+        <f t="shared" si="0"/>
+        <v>35</v>
       </c>
     </row>
     <row r="980" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -26462,11 +26547,12 @@
       <c r="D980" t="s">
         <v>27</v>
       </c>
-      <c r="E980" t="s">
-        <v>2088</v>
-      </c>
-      <c r="F980" t="s">
-        <v>2088</v>
+      <c r="E980">
+        <v>160</v>
+      </c>
+      <c r="F980">
+        <f t="shared" si="0"/>
+        <v>160</v>
       </c>
     </row>
     <row r="981" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -26482,11 +26568,12 @@
       <c r="D981" t="s">
         <v>27</v>
       </c>
-      <c r="E981" t="s">
-        <v>2088</v>
-      </c>
-      <c r="F981" t="s">
-        <v>2088</v>
+      <c r="E981">
+        <v>300</v>
+      </c>
+      <c r="F981">
+        <f t="shared" si="0"/>
+        <v>300</v>
       </c>
     </row>
     <row r="982" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -26502,11 +26589,12 @@
       <c r="D982" t="s">
         <v>27</v>
       </c>
-      <c r="E982" t="s">
-        <v>2088</v>
-      </c>
-      <c r="F982" t="s">
-        <v>2088</v>
+      <c r="E982">
+        <v>280</v>
+      </c>
+      <c r="F982">
+        <f t="shared" si="0"/>
+        <v>280</v>
       </c>
     </row>
     <row r="983" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -26525,8 +26613,9 @@
       <c r="E983" t="s">
         <v>2087</v>
       </c>
-      <c r="F983" t="s">
-        <v>2087</v>
+      <c r="F983" t="str">
+        <f t="shared" si="0"/>
+        <v>14</v>
       </c>
     </row>
     <row r="984" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -26542,11 +26631,12 @@
       <c r="D984" t="s">
         <v>2091</v>
       </c>
-      <c r="E984" t="s">
-        <v>2088</v>
-      </c>
-      <c r="F984" t="s">
-        <v>2088</v>
+      <c r="E984">
+        <v>50</v>
+      </c>
+      <c r="F984">
+        <f t="shared" si="0"/>
+        <v>50</v>
       </c>
     </row>
     <row r="985" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -26562,11 +26652,12 @@
       <c r="D985" t="s">
         <v>27</v>
       </c>
-      <c r="E985" t="s">
-        <v>2088</v>
-      </c>
-      <c r="F985" t="s">
-        <v>2088</v>
+      <c r="E985">
+        <v>178</v>
+      </c>
+      <c r="F985">
+        <f t="shared" si="0"/>
+        <v>178</v>
       </c>
     </row>
     <row r="986" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -26585,8 +26676,9 @@
       <c r="E986" t="s">
         <v>2089</v>
       </c>
-      <c r="F986" t="s">
-        <v>2089</v>
+      <c r="F986" t="str">
+        <f t="shared" si="0"/>
+        <v>10</v>
       </c>
     </row>
     <row r="987" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -26602,11 +26694,12 @@
       <c r="D987" t="s">
         <v>2091</v>
       </c>
-      <c r="E987" t="s">
-        <v>2088</v>
-      </c>
-      <c r="F987" t="s">
-        <v>2088</v>
+      <c r="E987">
+        <v>40</v>
+      </c>
+      <c r="F987">
+        <f t="shared" ref="F987:F992" si="1">E987</f>
+        <v>40</v>
       </c>
     </row>
     <row r="988" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -26625,8 +26718,9 @@
       <c r="E988" t="s">
         <v>2090</v>
       </c>
-      <c r="F988" t="s">
-        <v>2090</v>
+      <c r="F988" t="str">
+        <f t="shared" si="1"/>
+        <v>20</v>
       </c>
     </row>
     <row r="989" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -26645,8 +26739,9 @@
       <c r="E989" t="s">
         <v>2093</v>
       </c>
-      <c r="F989" t="s">
-        <v>2093</v>
+      <c r="F989" t="str">
+        <f t="shared" si="1"/>
+        <v>12</v>
       </c>
     </row>
     <row r="990" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -26665,8 +26760,9 @@
       <c r="E990" t="s">
         <v>2089</v>
       </c>
-      <c r="F990" t="s">
-        <v>2089</v>
+      <c r="F990" t="str">
+        <f t="shared" si="1"/>
+        <v>10</v>
       </c>
     </row>
     <row r="991" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -26685,8 +26781,9 @@
       <c r="E991" t="s">
         <v>2090</v>
       </c>
-      <c r="F991" t="s">
-        <v>2090</v>
+      <c r="F991" t="str">
+        <f t="shared" si="1"/>
+        <v>20</v>
       </c>
     </row>
     <row r="992" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -26705,8 +26802,9 @@
       <c r="E992" t="s">
         <v>2089</v>
       </c>
-      <c r="F992" t="s">
-        <v>2089</v>
+      <c r="F992" t="str">
+        <f t="shared" si="1"/>
+        <v>10</v>
       </c>
     </row>
     <row r="993" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -26725,8 +26823,9 @@
       <c r="E993" t="s">
         <v>2090</v>
       </c>
-      <c r="F993" t="s">
-        <v>2090</v>
+      <c r="F993" t="str">
+        <f>E993</f>
+        <v>20</v>
       </c>
     </row>
     <row r="994" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -26745,8 +26844,9 @@
       <c r="E994" t="s">
         <v>2090</v>
       </c>
-      <c r="F994" t="s">
-        <v>2090</v>
+      <c r="F994" t="str">
+        <f t="shared" ref="F994:F1010" si="2">E994</f>
+        <v>20</v>
       </c>
     </row>
     <row r="995" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -26765,8 +26865,9 @@
       <c r="E995" t="s">
         <v>2089</v>
       </c>
-      <c r="F995" t="s">
-        <v>2089</v>
+      <c r="F995" t="str">
+        <f t="shared" si="2"/>
+        <v>10</v>
       </c>
     </row>
     <row r="996" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -26785,8 +26886,9 @@
       <c r="E996" t="s">
         <v>2090</v>
       </c>
-      <c r="F996" t="s">
-        <v>2090</v>
+      <c r="F996" t="str">
+        <f t="shared" si="2"/>
+        <v>20</v>
       </c>
     </row>
     <row r="997" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -26805,8 +26907,9 @@
       <c r="E997" t="s">
         <v>2090</v>
       </c>
-      <c r="F997" t="s">
-        <v>2090</v>
+      <c r="F997" t="str">
+        <f t="shared" si="2"/>
+        <v>20</v>
       </c>
     </row>
     <row r="998" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -26825,8 +26928,9 @@
       <c r="E998" t="s">
         <v>2089</v>
       </c>
-      <c r="F998" t="s">
-        <v>2089</v>
+      <c r="F998" t="str">
+        <f t="shared" si="2"/>
+        <v>10</v>
       </c>
     </row>
     <row r="999" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -26845,8 +26949,9 @@
       <c r="E999" t="s">
         <v>2089</v>
       </c>
-      <c r="F999" t="s">
-        <v>2089</v>
+      <c r="F999" t="str">
+        <f t="shared" si="2"/>
+        <v>10</v>
       </c>
     </row>
     <row r="1000" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -26865,8 +26970,9 @@
       <c r="E1000" t="s">
         <v>2090</v>
       </c>
-      <c r="F1000" t="s">
-        <v>2090</v>
+      <c r="F1000" t="str">
+        <f t="shared" si="2"/>
+        <v>20</v>
       </c>
     </row>
     <row r="1001" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -26885,8 +26991,9 @@
       <c r="E1001" t="s">
         <v>2089</v>
       </c>
-      <c r="F1001" t="s">
-        <v>2089</v>
+      <c r="F1001" t="str">
+        <f t="shared" si="2"/>
+        <v>10</v>
       </c>
     </row>
     <row r="1002" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -26902,11 +27009,12 @@
       <c r="D1002" t="s">
         <v>2084</v>
       </c>
-      <c r="E1002" t="s">
-        <v>2088</v>
-      </c>
-      <c r="F1002" t="s">
-        <v>2088</v>
+      <c r="E1002">
+        <v>15</v>
+      </c>
+      <c r="F1002">
+        <f t="shared" si="2"/>
+        <v>15</v>
       </c>
     </row>
     <row r="1003" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -26922,11 +27030,12 @@
       <c r="D1003" t="s">
         <v>2088</v>
       </c>
-      <c r="E1003" t="s">
-        <v>2088</v>
-      </c>
-      <c r="F1003" t="s">
-        <v>2088</v>
+      <c r="E1003">
+        <v>309</v>
+      </c>
+      <c r="F1003">
+        <f t="shared" si="2"/>
+        <v>309</v>
       </c>
     </row>
     <row r="1004" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -26945,8 +27054,9 @@
       <c r="E1004" t="s">
         <v>2086</v>
       </c>
-      <c r="F1004" t="s">
-        <v>2086</v>
+      <c r="F1004" t="str">
+        <f t="shared" si="2"/>
+        <v>250</v>
       </c>
     </row>
     <row r="1005" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -26965,8 +27075,9 @@
       <c r="E1005" t="s">
         <v>2086</v>
       </c>
-      <c r="F1005" t="s">
-        <v>2086</v>
+      <c r="F1005" t="str">
+        <f t="shared" si="2"/>
+        <v>250</v>
       </c>
     </row>
     <row r="1006" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -26982,11 +27093,12 @@
       <c r="D1006" t="s">
         <v>2084</v>
       </c>
-      <c r="E1006" t="s">
-        <v>2088</v>
-      </c>
-      <c r="F1006" t="s">
-        <v>2088</v>
+      <c r="E1006">
+        <v>22</v>
+      </c>
+      <c r="F1006">
+        <f t="shared" si="2"/>
+        <v>22</v>
       </c>
     </row>
     <row r="1007" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -27002,11 +27114,12 @@
       <c r="D1007" t="s">
         <v>2084</v>
       </c>
-      <c r="E1007" t="s">
-        <v>2088</v>
-      </c>
-      <c r="F1007" t="s">
-        <v>2088</v>
+      <c r="E1007">
+        <v>22</v>
+      </c>
+      <c r="F1007">
+        <f t="shared" si="2"/>
+        <v>22</v>
       </c>
     </row>
     <row r="1008" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -27022,11 +27135,12 @@
       <c r="D1008" t="s">
         <v>2084</v>
       </c>
-      <c r="E1008" t="s">
-        <v>2088</v>
-      </c>
-      <c r="F1008" t="s">
-        <v>2088</v>
+      <c r="E1008">
+        <v>16</v>
+      </c>
+      <c r="F1008">
+        <f t="shared" si="2"/>
+        <v>16</v>
       </c>
     </row>
     <row r="1009" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -27042,11 +27156,12 @@
       <c r="D1009" t="s">
         <v>2084</v>
       </c>
-      <c r="E1009" t="s">
-        <v>2088</v>
-      </c>
-      <c r="F1009" t="s">
-        <v>2088</v>
+      <c r="E1009">
+        <v>16</v>
+      </c>
+      <c r="F1009">
+        <f t="shared" si="2"/>
+        <v>16</v>
       </c>
     </row>
     <row r="1010" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -27062,11 +27177,12 @@
       <c r="D1010" t="s">
         <v>2084</v>
       </c>
-      <c r="E1010" t="s">
-        <v>2088</v>
-      </c>
-      <c r="F1010" t="s">
-        <v>2088</v>
+      <c r="E1010">
+        <v>15</v>
+      </c>
+      <c r="F1010">
+        <f t="shared" si="2"/>
+        <v>15</v>
       </c>
     </row>
     <row r="1011" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -27083,10 +27199,11 @@
         <v>2084</v>
       </c>
       <c r="E1011" t="s">
-        <v>2088</v>
-      </c>
-      <c r="F1011" t="s">
-        <v>2088</v>
+        <v>2097</v>
+      </c>
+      <c r="F1011" t="str">
+        <f>E1011</f>
+        <v>17KG/CAN (LUTENSOL ON60</v>
       </c>
     </row>
     <row r="1012" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -27102,11 +27219,12 @@
       <c r="D1012" t="s">
         <v>2084</v>
       </c>
-      <c r="E1012" t="s">
-        <v>2088</v>
-      </c>
-      <c r="F1012" t="s">
-        <v>2088</v>
+      <c r="E1012">
+        <v>25</v>
+      </c>
+      <c r="F1012">
+        <f t="shared" ref="F1012:F1031" si="3">E1012</f>
+        <v>25</v>
       </c>
     </row>
     <row r="1013" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -27122,11 +27240,12 @@
       <c r="D1013" t="s">
         <v>2091</v>
       </c>
-      <c r="E1013" t="s">
-        <v>2088</v>
-      </c>
-      <c r="F1013" t="s">
-        <v>2088</v>
+      <c r="E1013">
+        <v>25</v>
+      </c>
+      <c r="F1013">
+        <f t="shared" si="3"/>
+        <v>25</v>
       </c>
     </row>
     <row r="1014" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -27142,11 +27261,12 @@
       <c r="D1014" t="s">
         <v>2091</v>
       </c>
-      <c r="E1014" t="s">
-        <v>2088</v>
-      </c>
-      <c r="F1014" t="s">
-        <v>2088</v>
+      <c r="E1014">
+        <v>500</v>
+      </c>
+      <c r="F1014">
+        <f t="shared" si="3"/>
+        <v>500</v>
       </c>
     </row>
     <row r="1015" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -27165,8 +27285,9 @@
       <c r="E1015" t="s">
         <v>2085</v>
       </c>
-      <c r="F1015" t="s">
-        <v>2085</v>
+      <c r="F1015" t="str">
+        <f t="shared" si="3"/>
+        <v>1200</v>
       </c>
     </row>
     <row r="1016" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -27182,11 +27303,12 @@
       <c r="D1016" t="s">
         <v>2091</v>
       </c>
-      <c r="E1016" t="s">
-        <v>2088</v>
-      </c>
-      <c r="F1016" t="s">
-        <v>2088</v>
+      <c r="E1016">
+        <v>25</v>
+      </c>
+      <c r="F1016">
+        <f t="shared" si="3"/>
+        <v>25</v>
       </c>
     </row>
     <row r="1017" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -27202,11 +27324,12 @@
       <c r="D1017" t="s">
         <v>2091</v>
       </c>
-      <c r="E1017" t="s">
-        <v>2088</v>
-      </c>
-      <c r="F1017" t="s">
-        <v>2088</v>
+      <c r="E1017">
+        <v>25</v>
+      </c>
+      <c r="F1017">
+        <f t="shared" si="3"/>
+        <v>25</v>
       </c>
     </row>
     <row r="1018" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -27225,8 +27348,9 @@
       <c r="E1018" t="s">
         <v>2090</v>
       </c>
-      <c r="F1018" t="s">
-        <v>2090</v>
+      <c r="F1018" t="str">
+        <f t="shared" si="3"/>
+        <v>20</v>
       </c>
     </row>
     <row r="1019" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -27245,8 +27369,9 @@
       <c r="E1019" t="s">
         <v>2090</v>
       </c>
-      <c r="F1019" t="s">
-        <v>2090</v>
+      <c r="F1019" t="str">
+        <f t="shared" si="3"/>
+        <v>20</v>
       </c>
     </row>
     <row r="1020" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -27265,8 +27390,9 @@
       <c r="E1020" t="s">
         <v>2090</v>
       </c>
-      <c r="F1020" t="s">
-        <v>2090</v>
+      <c r="F1020" t="str">
+        <f t="shared" si="3"/>
+        <v>20</v>
       </c>
     </row>
     <row r="1021" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -27285,8 +27411,9 @@
       <c r="E1021" t="s">
         <v>2089</v>
       </c>
-      <c r="F1021" t="s">
-        <v>2089</v>
+      <c r="F1021" t="str">
+        <f t="shared" si="3"/>
+        <v>10</v>
       </c>
     </row>
     <row r="1022" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -27302,11 +27429,12 @@
       <c r="D1022" t="s">
         <v>2083</v>
       </c>
-      <c r="E1022" t="s">
-        <v>2088</v>
-      </c>
-      <c r="F1022" t="s">
-        <v>2088</v>
+      <c r="E1022">
+        <v>380</v>
+      </c>
+      <c r="F1022">
+        <f t="shared" si="3"/>
+        <v>380</v>
       </c>
     </row>
     <row r="1023" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -27325,8 +27453,9 @@
       <c r="E1023" t="s">
         <v>2089</v>
       </c>
-      <c r="F1023" t="s">
-        <v>2089</v>
+      <c r="F1023" t="str">
+        <f t="shared" si="3"/>
+        <v>10</v>
       </c>
     </row>
     <row r="1024" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -27345,8 +27474,9 @@
       <c r="E1024" t="s">
         <v>2090</v>
       </c>
-      <c r="F1024" t="s">
-        <v>2090</v>
+      <c r="F1024" t="str">
+        <f t="shared" si="3"/>
+        <v>20</v>
       </c>
     </row>
     <row r="1025" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -27365,8 +27495,9 @@
       <c r="E1025" t="s">
         <v>2090</v>
       </c>
-      <c r="F1025" t="s">
-        <v>2090</v>
+      <c r="F1025" t="str">
+        <f t="shared" si="3"/>
+        <v>20</v>
       </c>
     </row>
     <row r="1026" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -27385,8 +27516,9 @@
       <c r="E1026" t="s">
         <v>2090</v>
       </c>
-      <c r="F1026" t="s">
-        <v>2090</v>
+      <c r="F1026" t="str">
+        <f t="shared" si="3"/>
+        <v>20</v>
       </c>
     </row>
     <row r="1027" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -27405,8 +27537,9 @@
       <c r="E1027" t="s">
         <v>2090</v>
       </c>
-      <c r="F1027" t="s">
-        <v>2090</v>
+      <c r="F1027" t="str">
+        <f t="shared" si="3"/>
+        <v>20</v>
       </c>
     </row>
     <row r="1028" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -27425,8 +27558,9 @@
       <c r="E1028" t="s">
         <v>2090</v>
       </c>
-      <c r="F1028" t="s">
-        <v>2090</v>
+      <c r="F1028" t="str">
+        <f t="shared" si="3"/>
+        <v>20</v>
       </c>
     </row>
     <row r="1029" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -27445,8 +27579,9 @@
       <c r="E1029" t="s">
         <v>2090</v>
       </c>
-      <c r="F1029" t="s">
-        <v>2090</v>
+      <c r="F1029" t="str">
+        <f t="shared" si="3"/>
+        <v>20</v>
       </c>
     </row>
     <row r="1030" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -27465,8 +27600,9 @@
       <c r="E1030" t="s">
         <v>2090</v>
       </c>
-      <c r="F1030" t="s">
-        <v>2090</v>
+      <c r="F1030" t="str">
+        <f t="shared" si="3"/>
+        <v>20</v>
       </c>
     </row>
     <row r="1031" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -27485,8 +27621,9 @@
       <c r="E1031" t="s">
         <v>2090</v>
       </c>
-      <c r="F1031" t="s">
-        <v>2090</v>
+      <c r="F1031" t="str">
+        <f t="shared" si="3"/>
+        <v>20</v>
       </c>
     </row>
     <row r="1032" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -27505,8 +27642,9 @@
       <c r="E1032" t="s">
         <v>2090</v>
       </c>
-      <c r="F1032" t="s">
-        <v>2090</v>
+      <c r="F1032" t="str">
+        <f>E1032</f>
+        <v>20</v>
       </c>
     </row>
     <row r="1033" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -27525,8 +27663,9 @@
       <c r="E1033" t="s">
         <v>2090</v>
       </c>
-      <c r="F1033" t="s">
-        <v>2090</v>
+      <c r="F1033" t="str">
+        <f t="shared" ref="F1033:F1091" si="4">E1033</f>
+        <v>20</v>
       </c>
     </row>
     <row r="1034" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -27542,11 +27681,9 @@
       <c r="D1034" t="s">
         <v>2088</v>
       </c>
-      <c r="E1034" t="s">
-        <v>2088</v>
-      </c>
-      <c r="F1034" t="s">
-        <v>2088</v>
+      <c r="F1034">
+        <f t="shared" si="4"/>
+        <v>0</v>
       </c>
     </row>
     <row r="1035" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -27562,11 +27699,12 @@
       <c r="D1035" t="s">
         <v>2091</v>
       </c>
-      <c r="E1035" t="s">
-        <v>2088</v>
-      </c>
-      <c r="F1035" t="s">
-        <v>2088</v>
+      <c r="E1035">
+        <v>25</v>
+      </c>
+      <c r="F1035">
+        <f t="shared" si="4"/>
+        <v>25</v>
       </c>
     </row>
     <row r="1036" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -27582,11 +27720,12 @@
       <c r="D1036" t="s">
         <v>2091</v>
       </c>
-      <c r="E1036" t="s">
-        <v>2088</v>
-      </c>
-      <c r="F1036" t="s">
-        <v>2088</v>
+      <c r="E1036">
+        <v>25</v>
+      </c>
+      <c r="F1036">
+        <f t="shared" si="4"/>
+        <v>25</v>
       </c>
     </row>
     <row r="1037" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -27602,11 +27741,12 @@
       <c r="D1037" t="s">
         <v>2091</v>
       </c>
-      <c r="E1037" t="s">
-        <v>2088</v>
-      </c>
-      <c r="F1037" t="s">
-        <v>2088</v>
+      <c r="E1037">
+        <v>50</v>
+      </c>
+      <c r="F1037">
+        <f t="shared" si="4"/>
+        <v>50</v>
       </c>
     </row>
     <row r="1038" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -27622,11 +27762,12 @@
       <c r="D1038" t="s">
         <v>2084</v>
       </c>
-      <c r="E1038" t="s">
-        <v>2088</v>
-      </c>
-      <c r="F1038" t="s">
-        <v>2088</v>
+      <c r="E1038">
+        <v>30</v>
+      </c>
+      <c r="F1038">
+        <f t="shared" si="4"/>
+        <v>30</v>
       </c>
     </row>
     <row r="1039" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -27642,11 +27783,12 @@
       <c r="D1039" t="s">
         <v>2084</v>
       </c>
-      <c r="E1039" t="s">
-        <v>2088</v>
-      </c>
-      <c r="F1039" t="s">
-        <v>2088</v>
+      <c r="E1039">
+        <v>25</v>
+      </c>
+      <c r="F1039">
+        <f t="shared" si="4"/>
+        <v>25</v>
       </c>
     </row>
     <row r="1040" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -27665,8 +27807,9 @@
       <c r="E1040" t="s">
         <v>2090</v>
       </c>
-      <c r="F1040" t="s">
-        <v>2090</v>
+      <c r="F1040" t="str">
+        <f t="shared" si="4"/>
+        <v>20</v>
       </c>
     </row>
     <row r="1041" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -27685,8 +27828,9 @@
       <c r="E1041" t="s">
         <v>2090</v>
       </c>
-      <c r="F1041" t="s">
-        <v>2090</v>
+      <c r="F1041" t="str">
+        <f t="shared" si="4"/>
+        <v>20</v>
       </c>
     </row>
     <row r="1042" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -27705,8 +27849,9 @@
       <c r="E1042" t="s">
         <v>2090</v>
       </c>
-      <c r="F1042" t="s">
-        <v>2090</v>
+      <c r="F1042" t="str">
+        <f t="shared" si="4"/>
+        <v>20</v>
       </c>
     </row>
     <row r="1043" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -27725,8 +27870,9 @@
       <c r="E1043" t="s">
         <v>2090</v>
       </c>
-      <c r="F1043" t="s">
-        <v>2090</v>
+      <c r="F1043" t="str">
+        <f t="shared" si="4"/>
+        <v>20</v>
       </c>
     </row>
     <row r="1044" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -27742,11 +27888,12 @@
       <c r="D1044" t="s">
         <v>27</v>
       </c>
-      <c r="E1044" t="s">
-        <v>2088</v>
-      </c>
-      <c r="F1044" t="s">
-        <v>2088</v>
+      <c r="E1044">
+        <v>160</v>
+      </c>
+      <c r="F1044">
+        <f t="shared" si="4"/>
+        <v>160</v>
       </c>
     </row>
     <row r="1045" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -27762,11 +27909,12 @@
       <c r="D1045" t="s">
         <v>27</v>
       </c>
-      <c r="E1045" t="s">
-        <v>2088</v>
-      </c>
-      <c r="F1045" t="s">
-        <v>2088</v>
+      <c r="E1045">
+        <v>180</v>
+      </c>
+      <c r="F1045">
+        <f t="shared" si="4"/>
+        <v>180</v>
       </c>
     </row>
     <row r="1046" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -27783,10 +27931,11 @@
         <v>2083</v>
       </c>
       <c r="E1046" t="s">
-        <v>2088</v>
-      </c>
-      <c r="F1046" t="s">
-        <v>2088</v>
+        <v>2098</v>
+      </c>
+      <c r="F1046" t="str">
+        <f t="shared" si="4"/>
+        <v>METHANO</v>
       </c>
     </row>
     <row r="1047" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -27802,11 +27951,12 @@
       <c r="D1047" t="s">
         <v>27</v>
       </c>
-      <c r="E1047" t="s">
-        <v>2088</v>
-      </c>
-      <c r="F1047" t="s">
-        <v>2088</v>
+      <c r="E1047">
+        <v>165</v>
+      </c>
+      <c r="F1047">
+        <f t="shared" si="4"/>
+        <v>165</v>
       </c>
     </row>
     <row r="1048" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -27822,11 +27972,12 @@
       <c r="D1048" t="s">
         <v>27</v>
       </c>
-      <c r="E1048" t="s">
-        <v>2088</v>
-      </c>
-      <c r="F1048" t="s">
-        <v>2088</v>
+      <c r="E1048">
+        <v>179</v>
+      </c>
+      <c r="F1048">
+        <f t="shared" si="4"/>
+        <v>179</v>
       </c>
     </row>
     <row r="1049" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -27842,11 +27993,12 @@
       <c r="D1049" t="s">
         <v>27</v>
       </c>
-      <c r="E1049" t="s">
-        <v>2088</v>
-      </c>
-      <c r="F1049" t="s">
-        <v>2088</v>
+      <c r="E1049">
+        <v>179</v>
+      </c>
+      <c r="F1049">
+        <f t="shared" si="4"/>
+        <v>179</v>
       </c>
     </row>
     <row r="1050" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -27862,11 +28014,12 @@
       <c r="D1050" t="s">
         <v>27</v>
       </c>
-      <c r="E1050" t="s">
-        <v>2088</v>
-      </c>
-      <c r="F1050" t="s">
-        <v>2088</v>
+      <c r="E1050">
+        <v>190</v>
+      </c>
+      <c r="F1050">
+        <f t="shared" si="4"/>
+        <v>190</v>
       </c>
     </row>
     <row r="1051" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -27882,11 +28035,12 @@
       <c r="D1051" t="s">
         <v>27</v>
       </c>
-      <c r="E1051" t="s">
-        <v>2088</v>
-      </c>
-      <c r="F1051" t="s">
-        <v>2088</v>
+      <c r="E1051">
+        <v>225</v>
+      </c>
+      <c r="F1051">
+        <f t="shared" si="4"/>
+        <v>225</v>
       </c>
     </row>
     <row r="1052" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -27902,11 +28056,12 @@
       <c r="D1052" t="s">
         <v>27</v>
       </c>
-      <c r="E1052" t="s">
-        <v>2088</v>
-      </c>
-      <c r="F1052" t="s">
-        <v>2088</v>
+      <c r="E1052">
+        <v>190</v>
+      </c>
+      <c r="F1052">
+        <f t="shared" si="4"/>
+        <v>190</v>
       </c>
     </row>
     <row r="1053" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -27922,11 +28077,12 @@
       <c r="D1053" t="s">
         <v>2092</v>
       </c>
-      <c r="E1053" t="s">
-        <v>2088</v>
-      </c>
-      <c r="F1053" t="s">
-        <v>2088</v>
+      <c r="E1053">
+        <v>40</v>
+      </c>
+      <c r="F1053">
+        <f t="shared" si="4"/>
+        <v>40</v>
       </c>
     </row>
     <row r="1054" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -27942,11 +28098,12 @@
       <c r="D1054" t="s">
         <v>2092</v>
       </c>
-      <c r="E1054" t="s">
-        <v>2088</v>
-      </c>
-      <c r="F1054" t="s">
-        <v>2088</v>
+      <c r="E1054">
+        <v>40</v>
+      </c>
+      <c r="F1054">
+        <f t="shared" si="4"/>
+        <v>40</v>
       </c>
     </row>
     <row r="1055" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -27962,11 +28119,12 @@
       <c r="D1055" t="s">
         <v>2084</v>
       </c>
-      <c r="E1055" t="s">
-        <v>2088</v>
-      </c>
-      <c r="F1055" t="s">
-        <v>2088</v>
+      <c r="E1055">
+        <v>18</v>
+      </c>
+      <c r="F1055">
+        <f t="shared" si="4"/>
+        <v>18</v>
       </c>
     </row>
     <row r="1056" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -27985,8 +28143,9 @@
       <c r="E1056" t="s">
         <v>2090</v>
       </c>
-      <c r="F1056" t="s">
-        <v>2090</v>
+      <c r="F1056" t="str">
+        <f t="shared" si="4"/>
+        <v>20</v>
       </c>
     </row>
     <row r="1057" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -28005,8 +28164,9 @@
       <c r="E1057" t="s">
         <v>2087</v>
       </c>
-      <c r="F1057" t="s">
-        <v>2087</v>
+      <c r="F1057" t="str">
+        <f t="shared" si="4"/>
+        <v>14</v>
       </c>
     </row>
     <row r="1058" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -28022,11 +28182,12 @@
       <c r="D1058" t="s">
         <v>2092</v>
       </c>
-      <c r="E1058" t="s">
-        <v>2088</v>
-      </c>
-      <c r="F1058" t="s">
-        <v>2088</v>
+      <c r="E1058">
+        <v>18</v>
+      </c>
+      <c r="F1058">
+        <f t="shared" si="4"/>
+        <v>18</v>
       </c>
     </row>
     <row r="1059" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -28042,11 +28203,12 @@
       <c r="D1059" t="s">
         <v>27</v>
       </c>
-      <c r="E1059" t="s">
-        <v>2088</v>
-      </c>
-      <c r="F1059" t="s">
-        <v>2088</v>
+      <c r="E1059">
+        <v>190</v>
+      </c>
+      <c r="F1059">
+        <f t="shared" si="4"/>
+        <v>190</v>
       </c>
     </row>
     <row r="1060" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -28062,11 +28224,12 @@
       <c r="D1060" t="s">
         <v>27</v>
       </c>
-      <c r="E1060" t="s">
-        <v>2088</v>
-      </c>
-      <c r="F1060" t="s">
-        <v>2088</v>
+      <c r="E1060">
+        <v>180</v>
+      </c>
+      <c r="F1060">
+        <f t="shared" si="4"/>
+        <v>180</v>
       </c>
     </row>
     <row r="1061" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -28082,11 +28245,12 @@
       <c r="D1061" t="s">
         <v>27</v>
       </c>
-      <c r="E1061" t="s">
-        <v>2088</v>
-      </c>
-      <c r="F1061" t="s">
-        <v>2088</v>
+      <c r="E1061">
+        <v>180</v>
+      </c>
+      <c r="F1061">
+        <f>E1061</f>
+        <v>180</v>
       </c>
     </row>
     <row r="1062" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -28102,11 +28266,12 @@
       <c r="D1062" t="s">
         <v>27</v>
       </c>
-      <c r="E1062" t="s">
-        <v>2088</v>
-      </c>
-      <c r="F1062" t="s">
-        <v>2088</v>
+      <c r="E1062">
+        <v>180</v>
+      </c>
+      <c r="F1062">
+        <f t="shared" si="4"/>
+        <v>180</v>
       </c>
     </row>
     <row r="1063" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -28122,11 +28287,12 @@
       <c r="D1063" t="s">
         <v>2084</v>
       </c>
-      <c r="E1063" t="s">
-        <v>2088</v>
-      </c>
-      <c r="F1063" t="s">
-        <v>2088</v>
+      <c r="E1063">
+        <v>5</v>
+      </c>
+      <c r="F1063">
+        <f t="shared" si="4"/>
+        <v>5</v>
       </c>
     </row>
     <row r="1064" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -28145,8 +28311,9 @@
       <c r="E1064" t="s">
         <v>2090</v>
       </c>
-      <c r="F1064" t="s">
-        <v>2090</v>
+      <c r="F1064" t="str">
+        <f t="shared" si="4"/>
+        <v>20</v>
       </c>
     </row>
     <row r="1065" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -28162,11 +28329,12 @@
       <c r="D1065" t="s">
         <v>2091</v>
       </c>
-      <c r="E1065" t="s">
-        <v>2088</v>
-      </c>
-      <c r="F1065" t="s">
-        <v>2088</v>
+      <c r="E1065">
+        <v>50</v>
+      </c>
+      <c r="F1065">
+        <f t="shared" si="4"/>
+        <v>50</v>
       </c>
     </row>
     <row r="1066" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -28185,8 +28353,9 @@
       <c r="E1066" t="s">
         <v>2090</v>
       </c>
-      <c r="F1066" t="s">
-        <v>2090</v>
+      <c r="F1066" t="str">
+        <f t="shared" si="4"/>
+        <v>20</v>
       </c>
     </row>
     <row r="1067" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -28202,11 +28371,12 @@
       <c r="D1067" t="s">
         <v>2091</v>
       </c>
-      <c r="E1067" t="s">
-        <v>2088</v>
-      </c>
-      <c r="F1067" t="s">
-        <v>2088</v>
+      <c r="E1067">
+        <v>25</v>
+      </c>
+      <c r="F1067">
+        <f t="shared" si="4"/>
+        <v>25</v>
       </c>
     </row>
     <row r="1068" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -28225,8 +28395,9 @@
       <c r="E1068" t="s">
         <v>2090</v>
       </c>
-      <c r="F1068" t="s">
-        <v>2090</v>
+      <c r="F1068" t="str">
+        <f t="shared" si="4"/>
+        <v>20</v>
       </c>
     </row>
     <row r="1069" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -28245,8 +28416,9 @@
       <c r="E1069" t="s">
         <v>2090</v>
       </c>
-      <c r="F1069" t="s">
-        <v>2090</v>
+      <c r="F1069" t="str">
+        <f t="shared" si="4"/>
+        <v>20</v>
       </c>
     </row>
     <row r="1070" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -28262,11 +28434,12 @@
       <c r="D1070" t="s">
         <v>2091</v>
       </c>
-      <c r="E1070" t="s">
-        <v>2088</v>
-      </c>
-      <c r="F1070" t="s">
-        <v>2088</v>
+      <c r="E1070">
+        <v>25</v>
+      </c>
+      <c r="F1070">
+        <f t="shared" si="4"/>
+        <v>25</v>
       </c>
     </row>
     <row r="1071" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -28285,8 +28458,9 @@
       <c r="E1071" t="s">
         <v>2089</v>
       </c>
-      <c r="F1071" t="s">
-        <v>2089</v>
+      <c r="F1071" t="str">
+        <f t="shared" si="4"/>
+        <v>10</v>
       </c>
     </row>
     <row r="1072" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -28302,11 +28476,12 @@
       <c r="D1072" t="s">
         <v>2091</v>
       </c>
-      <c r="E1072" t="s">
-        <v>2088</v>
-      </c>
-      <c r="F1072" t="s">
-        <v>2088</v>
+      <c r="E1072">
+        <v>25</v>
+      </c>
+      <c r="F1072">
+        <f t="shared" si="4"/>
+        <v>25</v>
       </c>
     </row>
     <row r="1073" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -28322,11 +28497,12 @@
       <c r="D1073" t="s">
         <v>2088</v>
       </c>
-      <c r="E1073" t="s">
-        <v>2088</v>
-      </c>
-      <c r="F1073" t="s">
-        <v>2088</v>
+      <c r="E1073">
+        <v>15</v>
+      </c>
+      <c r="F1073">
+        <f t="shared" si="4"/>
+        <v>15</v>
       </c>
     </row>
     <row r="1074" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -28345,8 +28521,9 @@
       <c r="E1074" t="s">
         <v>2090</v>
       </c>
-      <c r="F1074" t="s">
-        <v>2090</v>
+      <c r="F1074" t="str">
+        <f t="shared" si="4"/>
+        <v>20</v>
       </c>
     </row>
     <row r="1075" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -28362,11 +28539,12 @@
       <c r="D1075" t="s">
         <v>2091</v>
       </c>
-      <c r="E1075" t="s">
-        <v>2088</v>
-      </c>
-      <c r="F1075" t="s">
-        <v>2088</v>
+      <c r="E1075">
+        <v>25</v>
+      </c>
+      <c r="F1075">
+        <f t="shared" si="4"/>
+        <v>25</v>
       </c>
     </row>
     <row r="1076" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -28383,10 +28561,11 @@
         <v>2088</v>
       </c>
       <c r="E1076" t="s">
-        <v>2088</v>
-      </c>
-      <c r="F1076" t="s">
-        <v>2088</v>
+        <v>2099</v>
+      </c>
+      <c r="F1076" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve">Dau </v>
       </c>
     </row>
     <row r="1077" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -28402,11 +28581,12 @@
       <c r="D1077" t="s">
         <v>2092</v>
       </c>
-      <c r="E1077" t="s">
-        <v>2088</v>
-      </c>
-      <c r="F1077" t="s">
-        <v>2088</v>
+      <c r="E1077">
+        <v>9</v>
+      </c>
+      <c r="F1077">
+        <f t="shared" si="4"/>
+        <v>9</v>
       </c>
     </row>
     <row r="1078" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -28425,8 +28605,9 @@
       <c r="E1078" t="s">
         <v>2086</v>
       </c>
-      <c r="F1078" t="s">
-        <v>2086</v>
+      <c r="F1078" t="str">
+        <f t="shared" si="4"/>
+        <v>250</v>
       </c>
     </row>
     <row r="1079" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -28445,8 +28626,9 @@
       <c r="E1079" t="s">
         <v>2086</v>
       </c>
-      <c r="F1079" t="s">
-        <v>2086</v>
+      <c r="F1079" t="str">
+        <f t="shared" si="4"/>
+        <v>250</v>
       </c>
     </row>
     <row r="1080" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -28462,11 +28644,12 @@
       <c r="D1080" t="s">
         <v>2092</v>
       </c>
-      <c r="E1080" t="s">
-        <v>2088</v>
-      </c>
-      <c r="F1080" t="s">
-        <v>2088</v>
+      <c r="E1080">
+        <v>5372</v>
+      </c>
+      <c r="F1080">
+        <f t="shared" si="4"/>
+        <v>5372</v>
       </c>
     </row>
     <row r="1081" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -28485,8 +28668,9 @@
       <c r="E1081" t="s">
         <v>2087</v>
       </c>
-      <c r="F1081" t="s">
-        <v>2087</v>
+      <c r="F1081" t="str">
+        <f t="shared" si="4"/>
+        <v>14</v>
       </c>
     </row>
     <row r="1082" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -28502,11 +28686,12 @@
       <c r="D1082" t="s">
         <v>2092</v>
       </c>
-      <c r="E1082" t="s">
-        <v>2088</v>
-      </c>
-      <c r="F1082" t="s">
-        <v>2088</v>
+      <c r="E1082">
+        <v>6021</v>
+      </c>
+      <c r="F1082">
+        <f t="shared" si="4"/>
+        <v>6021</v>
       </c>
     </row>
     <row r="1083" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -28522,11 +28707,12 @@
       <c r="D1083" t="s">
         <v>2092</v>
       </c>
-      <c r="E1083" t="s">
-        <v>2088</v>
-      </c>
-      <c r="F1083" t="s">
-        <v>2088</v>
+      <c r="E1083">
+        <v>118</v>
+      </c>
+      <c r="F1083">
+        <f t="shared" si="4"/>
+        <v>118</v>
       </c>
     </row>
     <row r="1084" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -28545,8 +28731,9 @@
       <c r="E1084" t="s">
         <v>2090</v>
       </c>
-      <c r="F1084" t="s">
-        <v>2090</v>
+      <c r="F1084" t="str">
+        <f t="shared" si="4"/>
+        <v>20</v>
       </c>
     </row>
     <row r="1085" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -28565,8 +28752,9 @@
       <c r="E1085" t="s">
         <v>2087</v>
       </c>
-      <c r="F1085" t="s">
-        <v>2087</v>
+      <c r="F1085" t="str">
+        <f t="shared" si="4"/>
+        <v>14</v>
       </c>
     </row>
     <row r="1086" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -28583,10 +28771,11 @@
         <v>2088</v>
       </c>
       <c r="E1086" t="s">
-        <v>2088</v>
-      </c>
-      <c r="F1086" t="s">
-        <v>2088</v>
+        <v>2100</v>
+      </c>
+      <c r="F1086" t="str">
+        <f>E1086</f>
+        <v xml:space="preserve"> POC701</v>
       </c>
     </row>
     <row r="1087" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -28603,10 +28792,11 @@
         <v>2088</v>
       </c>
       <c r="E1087" t="s">
-        <v>2088</v>
-      </c>
-      <c r="F1087" t="s">
-        <v>2088</v>
+        <v>2101</v>
+      </c>
+      <c r="F1087" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve"> POC702</v>
       </c>
     </row>
     <row r="1088" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -28623,10 +28813,11 @@
         <v>2088</v>
       </c>
       <c r="E1088" t="s">
-        <v>2088</v>
-      </c>
-      <c r="F1088" t="s">
-        <v>2088</v>
+        <v>2102</v>
+      </c>
+      <c r="F1088" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve"> POC703</v>
       </c>
     </row>
     <row r="1089" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -28643,10 +28834,11 @@
         <v>2088</v>
       </c>
       <c r="E1089" t="s">
-        <v>2088</v>
-      </c>
-      <c r="F1089" t="s">
-        <v>2088</v>
+        <v>2103</v>
+      </c>
+      <c r="F1089" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve"> POC704</v>
       </c>
     </row>
     <row r="1090" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -28663,10 +28855,11 @@
         <v>2088</v>
       </c>
       <c r="E1090" t="s">
-        <v>2088</v>
-      </c>
-      <c r="F1090" t="s">
-        <v>2088</v>
+        <v>2104</v>
+      </c>
+      <c r="F1090" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve"> POC705</v>
       </c>
     </row>
     <row r="1091" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -28683,19 +28876,17 @@
         <v>2088</v>
       </c>
       <c r="E1091" t="s">
-        <v>2088</v>
-      </c>
-      <c r="F1091" t="s">
-        <v>2088</v>
+        <v>2105</v>
+      </c>
+      <c r="F1091" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve"> POC706</v>
       </c>
     </row>
     <row r="1092" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D1092" t="s">
         <v>2088</v>
       </c>
-      <c r="E1092" t="s">
-        <v>2088</v>
-      </c>
       <c r="F1092" t="s">
         <v>2088</v>
       </c>
@@ -28704,9 +28895,6 @@
       <c r="D1093" t="s">
         <v>2088</v>
       </c>
-      <c r="E1093" t="s">
-        <v>2088</v>
-      </c>
       <c r="F1093" t="s">
         <v>2088</v>
       </c>
@@ -28715,9 +28903,6 @@
       <c r="D1094" t="s">
         <v>2088</v>
       </c>
-      <c r="E1094" t="s">
-        <v>2088</v>
-      </c>
       <c r="F1094" t="s">
         <v>2088</v>
       </c>
@@ -28726,9 +28911,6 @@
       <c r="D1095" t="s">
         <v>2088</v>
       </c>
-      <c r="E1095" t="s">
-        <v>2088</v>
-      </c>
       <c r="F1095" t="s">
         <v>2088</v>
       </c>
@@ -28737,18 +28919,12 @@
       <c r="D1096" t="s">
         <v>2088</v>
       </c>
-      <c r="E1096" t="s">
-        <v>2088</v>
-      </c>
       <c r="F1096" t="s">
         <v>2088</v>
       </c>
     </row>
     <row r="1097" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D1097" t="s">
-        <v>2088</v>
-      </c>
-      <c r="E1097" t="s">
         <v>2088</v>
       </c>
       <c r="F1097" t="s">
@@ -28774,7 +28950,7 @@
       <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
       <pageSetup paperSize="9" fitToWidth="0" fitToHeight="0" orientation="landscape" r:id="rId1"/>
       <headerFooter alignWithMargins="0"/>
-      <autoFilter ref="A2:F2" xr:uid="{7DA33475-D1AD-44E5-8332-DB343ACC05BA}"/>
+      <autoFilter ref="A2:F2" xr:uid="{51126C8A-C685-4A7A-9961-D00212B392C7}"/>
     </customSheetView>
   </customSheetViews>
   <mergeCells count="1">

</xml_diff>